<commit_message>
Archivos agregados: modelo orcad con simulaciones y los pdfs - Archivos modificados: Excel gastos
</commit_message>
<xml_diff>
--- a/Tp_Balanza/componentes.xlsx
+++ b/Tp_Balanza/componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FACULTAD\Materias--4to-2do\Sintesis de Redes Activas\sintesis_redes_activas\Tp_Balanza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33906B9-CB7B-4E9D-A7ED-837B5CA27939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E8660B-A98B-46BD-9386-6775A7A9590C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07CA5786-9CCB-48C7-B0CE-ECF759E88083}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Componentes</t>
   </si>
@@ -55,13 +55,85 @@
   </si>
   <si>
     <t>OPA336UJ</t>
+  </si>
+  <si>
+    <t>TOTAL 1 BALANZA:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Res. 1k </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,5%</t>
+    </r>
+  </si>
+  <si>
+    <t>RR1220P-102-D</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Res. 10k </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,1%</t>
+    </r>
+  </si>
+  <si>
+    <t>RNCF0603BTE10K0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Res. 9k </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>± 0,1%</t>
+    </r>
+  </si>
+  <si>
+    <t>RT0805BRE079KL</t>
+  </si>
+  <si>
+    <t>Microcontrolador</t>
+  </si>
+  <si>
+    <t>PIC32MK1024MCF064T-I/MR</t>
+  </si>
+  <si>
+    <t>Impresión PCB</t>
+  </si>
+  <si>
+    <t>Restantes</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +141,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -206,41 +302,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,16 +678,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC8291C-37B1-4786-819D-17C02AE5E9F4}">
-  <dimension ref="C3:H17"/>
+  <dimension ref="C3:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.88671875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
@@ -575,48 +696,48 @@
   <sheetData>
     <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="8"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="12">
         <v>13.12</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f>E6*1000</f>
         <v>13120</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>1000</v>
       </c>
       <c r="H6" s="1">
@@ -625,169 +746,192 @@
       </c>
     </row>
     <row r="7" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="12">
         <v>1.1200000000000001</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" ref="F7:F17" si="0">E7*1000</f>
+      <c r="F7" s="2">
+        <f t="shared" ref="F7:F13" si="0">E7*1000</f>
         <v>1120</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>1000</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7:H17" si="1">F7*G7</f>
+        <f t="shared" ref="H7:H13" si="1">F7*G7</f>
         <v>1120000</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3">
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1.848E-2</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>18.48</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3000</v>
+      </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>55440</v>
       </c>
     </row>
     <row r="9" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3">
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2000</v>
+      </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>112000</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3">
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="12">
+        <v>7.9670000000000005E-2</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>79.67</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1000</v>
+      </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>79670</v>
       </c>
     </row>
     <row r="11" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3">
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="12">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>8210</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1000</v>
+      </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8210000</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="5"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3">
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1000</v>
+      </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3">
+        <v>137000</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5">
+        <f>30-(E16/1000)</f>
+        <v>6.04589</v>
+      </c>
+      <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="1">
+        <v>6045.89</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1000</v>
+      </c>
+      <c r="H13" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
+        <v>6045890</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15">
+        <f>F6+2*F7+3*F8+2*F9+F10+F11+F12</f>
+        <v>23954.11</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="3:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="C16:D18"/>
+    <mergeCell ref="E16:G18"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -796,5 +940,6 @@
     <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
circuito con res equalizada - correcccion modelo OPAM
</commit_message>
<xml_diff>
--- a/Tp_Balanza/componentes.xlsx
+++ b/Tp_Balanza/componentes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FACULTAD\Materias--4to-2do\Sintesis de Redes Activas\sintesis_redes_activas\Tp_Balanza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E8660B-A98B-46BD-9386-6775A7A9590C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AFDB0D-2CEF-41D2-A43D-EC349F53ECC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07CA5786-9CCB-48C7-B0CE-ECF759E88083}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>OAMP</t>
   </si>
   <si>
-    <t>OPA336UJ</t>
-  </si>
-  <si>
     <t>TOTAL 1 BALANZA:</t>
   </si>
   <si>
@@ -125,13 +122,16 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>OPA336N</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -336,25 +336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -362,6 +344,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -681,7 +681,7 @@
   <dimension ref="C3:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,32 +696,32 @@
   <sheetData>
     <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="9"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3" t="s">
@@ -730,7 +730,7 @@
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="6">
         <v>13.12</v>
       </c>
       <c r="F6" s="2">
@@ -750,31 +750,31 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1.1200000000000001</v>
+        <v>21</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1.29</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ref="F7:F13" si="0">E7*1000</f>
-        <v>1120</v>
+        <v>1290</v>
       </c>
       <c r="G7" s="2">
         <v>1000</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H13" si="1">F7*G7</f>
-        <v>1120000</v>
+        <v>1290000</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="E8" s="6">
         <v>1.848E-2</v>
       </c>
       <c r="F8" s="2">
@@ -791,12 +791,12 @@
     </row>
     <row r="9" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="E9" s="6">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="F9" s="2">
@@ -813,12 +813,12 @@
     </row>
     <row r="10" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="E10" s="6">
         <v>7.9670000000000005E-2</v>
       </c>
       <c r="F10" s="2">
@@ -835,12 +835,12 @@
     </row>
     <row r="11" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="E11" s="6">
         <v>8.2100000000000009</v>
       </c>
       <c r="F11" s="2">
@@ -857,10 +857,10 @@
     </row>
     <row r="12" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2">
         <v>0.13700000000000001</v>
@@ -879,54 +879,54 @@
     </row>
     <row r="13" spans="3:8" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E13" s="5">
         <f>30-(E16/1000)</f>
-        <v>6.04589</v>
+        <v>5.7058900000000001</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>6045.89</v>
+        <v>5705.89</v>
       </c>
       <c r="G13" s="5">
         <v>1000</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="7">
         <f t="shared" si="1"/>
-        <v>6045890</v>
+        <v>5705890</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15">
+      <c r="C16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9">
         <f>F6+2*F7+3*F8+2*F9+F10+F11+F12</f>
-        <v>23954.11</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+        <v>24294.11</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="3:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
actualizacion con OAMP MAX4238/4239
</commit_message>
<xml_diff>
--- a/Tp_Balanza/componentes.xlsx
+++ b/Tp_Balanza/componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FACULTAD\Materias--4to-2do\Sintesis de Redes Activas\sintesis_redes_activas\Tp_Balanza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AFDB0D-2CEF-41D2-A43D-EC349F53ECC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEB2801-18BB-420B-AF6D-3CF389B4D810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{07CA5786-9CCB-48C7-B0CE-ECF759E88083}"/>
   </bookViews>
@@ -123,7 +123,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>OPA336N</t>
+    <t>MAX 4238/4239</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="C3:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,18 +753,18 @@
         <v>21</v>
       </c>
       <c r="E7" s="6">
-        <v>1.29</v>
+        <v>1.52</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ref="F7:F13" si="0">E7*1000</f>
-        <v>1290</v>
+        <v>1520</v>
       </c>
       <c r="G7" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H13" si="1">F7*G7</f>
-        <v>1290000</v>
+        <v>3040000</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -886,18 +886,18 @@
       </c>
       <c r="E13" s="5">
         <f>30-(E16/1000)</f>
-        <v>5.7058900000000001</v>
+        <v>5.2458899999999993</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>5705.89</v>
+        <v>5245.8899999999994</v>
       </c>
       <c r="G13" s="5">
         <v>1000</v>
       </c>
       <c r="H13" s="7">
         <f t="shared" si="1"/>
-        <v>5705890</v>
+        <v>5245889.9999999991</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -909,7 +909,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="9">
         <f>F6+2*F7+3*F8+2*F9+F10+F11+F12</f>
-        <v>24294.11</v>
+        <v>24754.11</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>

</xml_diff>